<commit_message>
- Intial for Nhathau report
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeNhaThau.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeNhaThau.xlsx
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" calcMode="manual"/>
+  <calcPr calcId="152511" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>BẢNG KÊ VẬN CHUYỂN</t>
   </si>
@@ -63,12 +63,6 @@
     <t>Khách hàng</t>
   </si>
   <si>
-    <t>Số HĐ nâng</t>
-  </si>
-  <si>
-    <t>Số HĐ hạ</t>
-  </si>
-  <si>
     <t>Ghi Chú</t>
   </si>
   <si>
@@ -81,21 +75,6 @@
     <t>Noi den</t>
   </si>
   <si>
-    <t>filter</t>
-  </si>
-  <si>
-    <t>nha thầu/hãng tàu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time </t>
-  </si>
-  <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
     <t>Khác</t>
   </si>
   <si>
@@ -105,9 +84,6 @@
     <t>${name}</t>
   </si>
   <si>
-    <t>{start}</t>
-  </si>
-  <si>
     <t>${end}</t>
   </si>
   <si>
@@ -120,9 +96,6 @@
     <t>${detail.jobNo}</t>
   </si>
   <si>
-    <t>${detail.date}</t>
-  </si>
-  <si>
     <t>${detail.cusName}</t>
   </si>
   <si>
@@ -156,24 +129,35 @@
     <t>${detail.phuthu}</t>
   </si>
   <si>
-    <t>${detail.sohdnang}</t>
-  </si>
-  <si>
-    <t>${detail.sohdHa}</t>
-  </si>
-  <si>
-    <t>${detail.note}</t>
+    <t>${detail.dateDev}</t>
+  </si>
+  <si>
+    <t>${start}</t>
+  </si>
+  <si>
+    <t>${detail.index}</t>
+  </si>
+  <si>
+    <t>&lt;/jx:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${feeNames}" var="feeName"&gt;</t>
+  </si>
+  <si>
+    <t>${feeName}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,8 +222,16 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +241,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,7 +331,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -361,12 +359,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -374,17 +366,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -734,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,87 +753,86 @@
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="13" max="16" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:19" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
     </row>
-    <row r="2" spans="1:18" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
+    <row r="2" spans="1:19" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="M2" s="13"/>
       <c r="N2" s="15"/>
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
     </row>
-    <row r="3" spans="1:18" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>25</v>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="19"/>
+      <c r="J3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="19"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="14"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -840,13 +843,14 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -878,88 +882,87 @@
         <v>7</v>
       </c>
       <c r="K5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="P5" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>14</v>
-      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="23"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" s="22">
+        <f>SUM(L6:Q6)</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="3"/>
     </row>
-    <row r="6" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>2</v>
-      </c>
+    <row r="7" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -977,382 +980,15 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
-    </row>
-    <row r="8" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-    </row>
-    <row r="9" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-    </row>
-    <row r="10" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-    </row>
-    <row r="11" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-    </row>
-    <row r="12" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-    </row>
-    <row r="13" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>8</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-    </row>
-    <row r="14" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-    </row>
-    <row r="15" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>10</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-    </row>
-    <row r="16" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>11</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-    </row>
-    <row r="17" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>12</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-    </row>
-    <row r="18" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>13</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-    </row>
-    <row r="19" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>14</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-    </row>
-    <row r="20" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>15</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-    </row>
-    <row r="21" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>16</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-    </row>
-    <row r="22" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>17</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-    </row>
-    <row r="23" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>18</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" t="s">
-        <v>22</v>
-      </c>
+      <c r="S7" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="A1:R1"/>
+  <mergeCells count="5">
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Dynamic col for fee
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeNhaThau.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeNhaThau.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>BẢNG KÊ VẬN CHUYỂN</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>${feeName}</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${detail.convertedFee}" var="feeVal"&gt;</t>
+  </si>
+  <si>
+    <t>${feeVal}</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${details}" var="detail"&gt;</t>
   </si>
 </sst>
 </file>
@@ -375,20 +384,20 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -738,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,27 +766,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
     </row>
     <row r="2" spans="1:19" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
@@ -810,18 +819,18 @@
       <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="18" t="s">
+      <c r="I3" s="23"/>
+      <c r="J3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="19" t="s">
+      <c r="K3" s="22"/>
+      <c r="L3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="19"/>
+      <c r="M3" s="23"/>
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
@@ -846,8 +855,8 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -910,77 +919,108 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6" s="23"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="22">
-        <f>SUM(L6:Q6)</f>
-        <v>0</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
       <c r="S6" s="3"/>
     </row>
     <row r="7" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="R7" s="19">
+        <f>SUM(L7:Q7)</f>
+        <v>0</v>
+      </c>
       <c r="S7" s="3"/>
+    </row>
+    <row r="8" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>